<commit_message>
updated summary stats file names
</commit_message>
<xml_diff>
--- a/dataset_metadata/discarded_datasets_summary.xlsx
+++ b/dataset_metadata/discarded_datasets_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>Has Raw Counts</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Size (GB)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -472,6 +477,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -490,6 +496,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -508,6 +515,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -526,6 +534,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -544,6 +553,7 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -561,6 +571,46 @@
         <is>
           <t>Yes</t>
         </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GasperiniShendure2019_atscale.h5ad</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>1.738121328875422</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>GasperiniShendure2019_highMOI.h5ad</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0.3896072432398796</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GasperiniShendure2019_lowMOI.h5ad</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>0.300553466193378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>